<commit_message>
The dictionary of mark dictionary has been finished.
</commit_message>
<xml_diff>
--- a/高考体育成绩对照表.xlsx
+++ b/高考体育成绩对照表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13470" windowHeight="6600"/>
+    <workbookView windowWidth="15240" windowHeight="4755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,9 +16,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6">
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="ˎ̥"/>
+        <charset val="0"/>
+      </rPr>
       <t>100</t>
     </r>
     <r>
@@ -27,23 +34,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="2"/>
         <charset val="0"/>
-      </rPr>
-      <t>米</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>100</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
       </rPr>
       <t>米</t>
     </r>
@@ -85,7 +76,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="ˎ̥"/>
-      <family val="2"/>
       <charset val="0"/>
     </font>
     <font>
@@ -100,7 +90,6 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="ˎ̥"/>
-      <family val="2"/>
       <charset val="0"/>
     </font>
     <font>
@@ -108,8 +97,22 @@
       <sz val="10.5"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
       <charset val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -122,6 +125,52 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -144,15 +193,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -175,21 +216,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -203,38 +237,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -249,25 +252,9 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="0"/>
     </font>
   </fonts>
@@ -280,37 +267,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -328,108 +303,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -442,7 +315,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,13 +411,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,11 +461,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,17 +515,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -537,32 +550,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -579,10 +566,10 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -591,133 +578,133 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1060,7 +1047,7 @@
   <dimension ref="B2:Q105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1084,29 +1071,27 @@
     <col min="17" max="17" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="30" spans="2:17">
+    <row r="2" ht="15.75" spans="2:17">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
@@ -1114,35 +1099,35 @@
     </row>
     <row r="3" customHeight="1" spans="2:17">
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q3" s="2"/>
     </row>

</xml_diff>

<commit_message>
PE mark can write to a excel file.
</commit_message>
<xml_diff>
--- a/高考体育成绩对照表.xlsx
+++ b/高考体育成绩对照表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15240" windowHeight="4755"/>
+    <workbookView windowWidth="14745" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -267,6 +267,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -291,6 +297,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -298,6 +310,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,13 +351,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -369,25 +405,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,43 +447,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -566,10 +566,10 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -578,16 +578,16 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -599,10 +599,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -623,28 +623,28 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -653,58 +653,58 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1047,7 +1047,7 @@
   <dimension ref="B2:Q105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>

</xml_diff>